<commit_message>
Adapted H2-balanced to run with updated NE: ini based on other scenarios, use of common hydro inputs, fixes made in H2 heavy branch.
</commit_message>
<xml_diff>
--- a/src_files/data_files/H2 balanced.xlsx
+++ b/src_files/data_files/H2 balanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backbone\north_european_model (2IMatch)\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFDFA18-6681-456A-B10E-6F59C831945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CD8FB1-F1F4-4A1B-99C5-E92A58ADA637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>elec</t>
-  </si>
-  <si>
-    <t>ETS_CO2</t>
   </si>
   <si>
     <t>Lignite</t>
@@ -732,6 +729,9 @@
       </rPr>
       <t>. The addition of such aspects represent significant modeling development effort without guarantee of provide scenario without unreastically large shortages. Instead, restoration of old capacities is chosen as the easiest option to balance scenario.</t>
     </r>
+  </si>
+  <si>
+    <t>ETS-CO2</t>
   </si>
 </sst>
 </file>
@@ -1600,7 +1600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4A9D05-A5A4-4554-9752-F0090415A662}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13:P14"/>
     </sheetView>
   </sheetViews>
@@ -1612,10 +1612,10 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="92" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" s="92" t="s">
-        <v>102</v>
       </c>
       <c r="C1" s="92"/>
       <c r="D1" s="92"/>
@@ -1635,7 +1635,7 @@
     <row r="2" spans="1:16">
       <c r="A2" s="92"/>
       <c r="B2" s="92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="92"/>
       <c r="D2" s="92"/>
@@ -1654,10 +1654,10 @@
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" s="91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="97"/>
       <c r="D3" s="97"/>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="91" t="s">
         <v>107</v>
-      </c>
-      <c r="B10" s="91" t="s">
-        <v>108</v>
       </c>
       <c r="C10" s="91"/>
       <c r="D10" s="91"/>
@@ -1807,7 +1807,7 @@
     <row r="11" spans="1:16">
       <c r="A11" s="91"/>
       <c r="B11" s="91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="91"/>
       <c r="D11" s="91"/>
@@ -1827,7 +1827,7 @@
     <row r="12" spans="1:16">
       <c r="A12" s="91"/>
       <c r="B12" s="91" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="91"/>
       <c r="D12" s="91"/>
@@ -1846,10 +1846,10 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="97" t="s">
         <v>110</v>
-      </c>
-      <c r="B13" s="97" t="s">
-        <v>111</v>
       </c>
       <c r="C13" s="97"/>
       <c r="D13" s="97"/>
@@ -2194,7 +2194,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>0</v>
@@ -3064,12 +3064,12 @@
   </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J63" sqref="J63"/>
       <selection pane="topRight" activeCell="J63" sqref="J63"/>
       <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
-      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -3144,10 +3144,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" s="82" t="s">
         <v>81</v>
@@ -3188,10 +3188,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G3" s="82" t="s">
         <v>81</v>
@@ -3232,10 +3232,10 @@
         <v>40</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" s="82" t="s">
         <v>81</v>
@@ -3276,13 +3276,13 @@
         <v>22</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="82" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="82" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>81</v>
@@ -3323,13 +3323,13 @@
         <v>37</v>
       </c>
       <c r="D6" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="82" t="s">
         <v>89</v>
-      </c>
-      <c r="E6" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="82" t="s">
-        <v>90</v>
       </c>
       <c r="G6" s="82" t="s">
         <v>81</v>
@@ -3422,10 +3422,10 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
@@ -5258,10 +5258,10 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -6527,7 +6527,7 @@
     </row>
     <row r="61" spans="1:23">
       <c r="A61" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>58</v>
@@ -6744,7 +6744,7 @@
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" s="70"/>
       <c r="C68" s="71"/>
@@ -9286,7 +9286,7 @@
     </row>
     <row r="103" spans="1:22">
       <c r="A103" s="73" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B103" s="74"/>
       <c r="C103" s="75"/>
@@ -12094,7 +12094,7 @@
     </row>
     <row r="139" spans="1:25">
       <c r="A139" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B139" s="34"/>
       <c r="C139" s="35"/>
@@ -15184,7 +15184,7 @@
     </row>
     <row r="175" spans="1:25">
       <c r="A175" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B175" s="34"/>
       <c r="C175" s="35"/>
@@ -15234,7 +15234,7 @@
         <v>53</v>
       </c>
       <c r="B177" s="53">
-        <f t="shared" ref="B177:C208" si="96">MAX(B70,B105)</f>
+        <f t="shared" ref="B177:C207" si="96">MAX(B70,B105)</f>
         <v>0</v>
       </c>
       <c r="C177" s="53">
@@ -15245,12 +15245,12 @@
         <v>18</v>
       </c>
       <c r="E177" s="53">
-        <f t="shared" ref="E177:E208" si="97">MAX(E70,E105)</f>
+        <f t="shared" ref="E177:E207" si="97">MAX(E70,E105)</f>
         <v>0</v>
       </c>
       <c r="F177" s="53"/>
       <c r="G177" s="53">
-        <f t="shared" ref="G177:H208" si="98">MAX(G70,G105)</f>
+        <f t="shared" ref="G177:H207" si="98">MAX(G70,G105)</f>
         <v>0</v>
       </c>
       <c r="H177" s="53">
@@ -15285,7 +15285,7 @@
         <v>0</v>
       </c>
       <c r="D178" s="8">
-        <f t="shared" ref="D178:D208" si="99">MAX(D71,D106)</f>
+        <f t="shared" ref="D178:D207" si="99">MAX(D71,D106)</f>
         <v>12</v>
       </c>
       <c r="E178" s="8">
@@ -16644,7 +16644,7 @@
     </row>
     <row r="209" spans="1:22">
       <c r="A209" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B209" s="15">
         <f>SUM(B177:B208)</f>
@@ -16694,7 +16694,7 @@
     </row>
     <row r="210" spans="1:22">
       <c r="A210" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B210" s="15">
         <f>B28</f>
@@ -16744,7 +16744,7 @@
     </row>
     <row r="211" spans="1:22">
       <c r="A211" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I211" s="98">
         <f>I209-I210</f>

</xml_diff>